<commit_message>
chaning to binary lotteries + analysis of survey
</commit_message>
<xml_diff>
--- a/flanker.xlsx
+++ b/flanker.xlsx
@@ -974,6 +974,12 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>2.111111111111111</v>
+      </c>
+      <c r="L2">
+        <v>0.3627294273273439</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
@@ -1006,6 +1012,12 @@
       <c r="J3">
         <v>1</v>
       </c>
+      <c r="K3">
+        <v>0.6170212765957447</v>
+      </c>
+      <c r="L3">
+        <v>0.8513141605137295</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
@@ -1266,6 +1278,12 @@
       <c r="J10">
         <v>1</v>
       </c>
+      <c r="K10">
+        <v>0.7297297297297298</v>
+      </c>
+      <c r="L10">
+        <v>0.7350839205477051</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
@@ -1350,6 +1368,12 @@
       <c r="J13">
         <v>1</v>
       </c>
+      <c r="K13">
+        <v>0.7</v>
+      </c>
+      <c r="L13">
+        <v>0.9888895391304537</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -1776,6 +1800,12 @@
       <c r="J25">
         <v>1</v>
       </c>
+      <c r="K25">
+        <v>1.095238095238096</v>
+      </c>
+      <c r="L25">
+        <v>0.9435952816082406</v>
+      </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
@@ -2064,6 +2094,12 @@
       <c r="J34">
         <v>1</v>
       </c>
+      <c r="K34">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="L34">
+        <v>0.8708550284809176</v>
+      </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
@@ -3236,6 +3272,12 @@
       <c r="J65">
         <v>1</v>
       </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>0.9979637820245348</v>
+      </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" t="s">
@@ -6109,6 +6151,12 @@
       </c>
       <c r="J143">
         <v>1</v>
+      </c>
+      <c r="K143">
+        <v>0.8181818181818181</v>
+      </c>
+      <c r="L143">
+        <v>0.8186376932720435</v>
       </c>
     </row>
     <row r="144" spans="1:12">

</xml_diff>